<commit_message>
cometa de la farola6
</commit_message>
<xml_diff>
--- a/archivo_descargado.xlsx
+++ b/archivo_descargado.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\.shortcut-targets-by-id\1ry4DW0ytzBTm2QpZbBJtiQ_i_FWgsO8E\Experimentos dECON\Curso_Experimentos WEB\Ediciones\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3D4E89C-4CCE-4D6E-8D1B-8EAAD285C320}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{880BEFB0-9137-4614-8D76-6C2A39C57822}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-24120" yWindow="-2655" windowWidth="24240" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -153,9 +153,6 @@
     <t>Experimentos de campo</t>
   </si>
   <si>
-    <t>[Tipos de Experimentos](https://drive.google.com/file/d/10A4EJFGWfebygOzYqxJxFSMew-zIN9r7/view?usp=sharing)</t>
-  </si>
-  <si>
     <t>Experimentos naturales</t>
   </si>
   <si>
@@ -208,6 +205,9 @@
   </si>
   <si>
     <t>Lab11: experimentos de laboratorio [.zip](https://drive.usercontent.google.com/u/1/uc?id=1tl7wGmp-MpVOC6SCJIX4wWr6kTbD6baR&amp;export=download)</t>
+  </si>
+  <si>
+    <t>[Tipos de Experimentos](https://drive.google.com/uc?id=10NvXg9FUUU0muewzUiHE0CgGXWOo_wpK&amp;export=download)</t>
   </si>
 </sst>
 </file>
@@ -948,8 +948,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -981,7 +981,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="36" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G1" s="6"/>
       <c r="H1" s="6"/>
@@ -1213,7 +1213,7 @@
         <v>14</v>
       </c>
       <c r="E8" s="14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F8" s="38"/>
       <c r="G8" s="6"/>
@@ -1311,13 +1311,13 @@
         <v>17</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E11" s="14" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F11" s="38" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G11" s="6"/>
       <c r="H11" s="6"/>
@@ -1355,7 +1355,7 @@
         <v>19</v>
       </c>
       <c r="E12" s="14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F12" s="38"/>
       <c r="G12" s="6"/>
@@ -1391,7 +1391,7 @@
         <v>20</v>
       </c>
       <c r="D13" s="17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E13" s="18" t="s">
         <v>21</v>
@@ -1461,7 +1461,7 @@
         <v>23</v>
       </c>
       <c r="D15" s="13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E15" s="14" t="s">
         <v>24</v>
@@ -1496,10 +1496,10 @@
         <v>25</v>
       </c>
       <c r="D16" s="28" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E16" s="29" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F16" s="41"/>
       <c r="G16" s="6"/>
@@ -1892,7 +1892,7 @@
         <v>41</v>
       </c>
       <c r="D28" s="13" t="s">
-        <v>42</v>
+        <v>60</v>
       </c>
       <c r="E28" s="14"/>
       <c r="F28" s="38"/>
@@ -1922,10 +1922,10 @@
       <c r="A29" s="11"/>
       <c r="B29" s="12"/>
       <c r="C29" s="13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D29" s="13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E29" s="14"/>
       <c r="F29" s="38"/>
@@ -1959,13 +1959,13 @@
         <v>45617</v>
       </c>
       <c r="C30" s="13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D30" s="13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E30" s="14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F30" s="38"/>
       <c r="G30" s="6"/>
@@ -1994,13 +1994,13 @@
       <c r="A31" s="15"/>
       <c r="B31" s="16"/>
       <c r="C31" s="17" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D31" s="17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E31" s="18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F31" s="39"/>
       <c r="G31" s="6"/>

</xml_diff>